<commit_message>
Latest push for 04Oct
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/colt/qa/datalibrary/APT_DDIRange.xlsx
+++ b/APTAutomationProject/src/com/colt/qa/datalibrary/APT_DDIRange.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APT_phase1_deliverable24082020\APTAutomationProject\src\com\colt\qa\datalibrary\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15780" windowHeight="3630"/>
   </bookViews>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
   <si>
     <t>TrunkValue</t>
   </si>
@@ -104,15 +99,12 @@
   </si>
   <si>
     <t>APT_VoiceService</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -294,7 +286,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -471,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -482,7 +474,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,7 +540,7 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>25</v>
@@ -601,7 +593,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +659,7 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>25</v>
@@ -711,7 +703,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>25</v>
@@ -764,7 +756,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +822,7 @@
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>25</v>
@@ -874,7 +866,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
All Modules- Merged Code
</commit_message>
<xml_diff>
--- a/APTAutomationProject/src/com/colt/qa/datalibrary/APT_DDIRange.xlsx
+++ b/APTAutomationProject/src/com/colt/qa/datalibrary/APT_DDIRange.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APT_Phase1_Automation_Project_Deliverables\APTAutomationProject\src\com\colt\qa\datalibrary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="5955"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="DDI" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -465,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>